<commit_message>
Fix variables used in matching
</commit_message>
<xml_diff>
--- a/databases/MedForm.xlsx
+++ b/databases/MedForm.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Einzeldosiertes Liquid</t>
   </si>
   <si>
-    <t xml:space="preserve">LT</t>
+    <t xml:space="preserve">Lt</t>
   </si>
   <si>
     <t xml:space="preserve">Lutschtablette</t>
@@ -298,10 +298,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.85"/>

</xml_diff>